<commit_message>
Updated test case files
</commit_message>
<xml_diff>
--- a/Test Cases/Test Cases.xlsx
+++ b/Test Cases/Test Cases.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="180">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Pass</t>
   </si>
   <si>
-    <t>missing: ac-5, ca-9, cm-8, ac-4</t>
-  </si>
-  <si>
     <t>AC-14</t>
   </si>
   <si>
@@ -118,7 +115,29 @@
     <t>Separation of Duties</t>
   </si>
   <si>
-    <t>https://nvd.nist.gov/800-53/Rev4/control/AC-5</t>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF000000"/>
+      </rPr>
+      <t>) Assign roles to table for anyone accessing database
+2) Create a username and password specific to each user</t>
+    </r>
+  </si>
+  <si>
+    <t>Admin should be able to log in with administrator priveleges</t>
+  </si>
+  <si>
+    <t>Admin is able to login</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
   <si>
     <t>AC-7</t>
@@ -163,9 +182,6 @@
   </si>
   <si>
     <t>"You are about to access crucial information and you're actions may be monitored. IF you wish to continue click ok."</t>
-  </si>
-  <si>
-    <t>PASS</t>
   </si>
   <si>
     <t>ac8</t>
@@ -195,7 +211,7 @@
     <t>Pass for 1/2 requirements</t>
   </si>
   <si>
-    <t>au8 1 and 2</t>
+    <t>au8 and ac-5 pic</t>
   </si>
   <si>
     <t>AT-4</t>
@@ -204,7 +220,13 @@
     <t>Security Training Records</t>
   </si>
   <si>
-    <t>Log in as a supervisor. Access the file for security training</t>
+    <t>Open documentation for policy AT-4</t>
+  </si>
+  <si>
+    <t>File is able to be opened</t>
+  </si>
+  <si>
+    <t>File opened</t>
   </si>
   <si>
     <t>CA-5</t>
@@ -214,12 +236,6 @@
   </si>
   <si>
     <t>Open documentation policy(ca-5)</t>
-  </si>
-  <si>
-    <t>File is able to be opened</t>
-  </si>
-  <si>
-    <t>File opened</t>
   </si>
   <si>
     <t>CA-7</t>
@@ -238,10 +254,16 @@
     <t xml:space="preserve">File is opened and guidelines followed </t>
   </si>
   <si>
-    <t>CA-9</t>
-  </si>
-  <si>
-    <t>Internal System Connections</t>
+    <t>PE-12</t>
+  </si>
+  <si>
+    <t>Emergency Lighting</t>
+  </si>
+  <si>
+    <t>Open documentation policy PE-12</t>
+  </si>
+  <si>
+    <t>File is opened and guidelines followed</t>
   </si>
   <si>
     <t>CM-10</t>
@@ -279,10 +301,13 @@
     <t>cm-7 pic</t>
   </si>
   <si>
-    <t>CM-8</t>
-  </si>
-  <si>
-    <t>Information System Component Inventory</t>
+    <t>CM-11</t>
+  </si>
+  <si>
+    <t>User Installed Software</t>
+  </si>
+  <si>
+    <t>Open documentation policy on CM-11</t>
   </si>
   <si>
     <t>CP-1</t>
@@ -300,7 +325,8 @@
     <t xml:space="preserve">Contingency Plan </t>
   </si>
   <si>
-    <t xml:space="preserve">Step 1: Develop a contigency plan that identifies essential business functions, provides recovery objectives, resoration priorities, and addresses maintaining these essential business functions
+    <t xml:space="preserve">Open documentation on CP-2
+Step 1: Develop a contigency plan that identifies essential business functions, provides recovery objectives, resoration priorities, and addresses maintaining these essential business functions
 </t>
   </si>
   <si>
@@ -563,7 +589,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="11">
+  <fonts count="12">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -611,6 +637,11 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="12.0"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <u/>
       <color rgb="FF1155CC"/>
       <name val="Arial"/>
@@ -642,7 +673,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border/>
     <border>
       <left style="thin">
@@ -666,11 +697,25 @@
         <color rgb="FF000000"/>
       </bottom>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -689,61 +734,58 @@
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
+    <xf borderId="3" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="2" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -766,7 +808,7 @@
     <xdr:ext cx="2705100" cy="2247900"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -794,7 +836,7 @@
     <xdr:ext cx="1819275" cy="1619250"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -822,7 +864,7 @@
     <xdr:ext cx="3086100" cy="2676525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image3.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -843,14 +885,14 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>676275</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2552700" cy="2914650"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -878,7 +920,7 @@
     <xdr:ext cx="5238750" cy="3886200"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image8.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -906,7 +948,7 @@
     <xdr:ext cx="2990850" cy="2447925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image2.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -934,7 +976,7 @@
     <xdr:ext cx="1343025" cy="2143125"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image4.png" title="Image"/>
+        <xdr:cNvPr id="0" name="image7.png" title="Image"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1240,445 +1282,492 @@
       <c r="G2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="6" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>17</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="9" t="s">
+      <c r="B4" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="D4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="F4" s="5" t="s">
         <v>24</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>25</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="C5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="D5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="E5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="G5" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="B6" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="H7" s="16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="K8" s="16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G10" s="14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B6" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="16" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>36</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="G7" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H7" s="17" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="K8" s="17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-    </row>
     <row r="11">
-      <c r="A11" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>64</v>
+      <c r="A11" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>67</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="G11" s="12" t="s">
+      <c r="E11" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F11" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="B12" s="20" t="s">
+      <c r="A12" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="B12" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="D12" s="21"/>
-      <c r="E12" s="8" t="s">
+      <c r="C12" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="D12" s="20"/>
+      <c r="E12" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="F12" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
+      <c r="B13" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>75</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="21" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="23"/>
+        <v>79</v>
+      </c>
+      <c r="D14" s="22"/>
       <c r="E14" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
+        <v>80</v>
+      </c>
+      <c r="F14" s="22"/>
+      <c r="G14" s="22"/>
     </row>
     <row r="15">
       <c r="A15" s="4" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C15" s="24" t="s">
-        <v>80</v>
+        <v>82</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>83</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="H15" s="17" t="s">
-        <v>84</v>
+        <v>36</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B16" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="22"/>
-      <c r="E16" s="22"/>
-      <c r="F16" s="22"/>
-      <c r="G16" s="22"/>
+      <c r="A16" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16" s="21" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="8" t="s">
-        <v>87</v>
-      </c>
-      <c r="B17" s="8" t="s">
-        <v>88</v>
-      </c>
-      <c r="C17" s="21" t="s">
-        <v>89</v>
+      <c r="A17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="20" t="s">
+        <v>93</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>66</v>
+      <c r="E17" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F17" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="23"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
+        <v>95</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19">
-      <c r="A19" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>95</v>
+      <c r="A19" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C19" s="16" t="s">
+        <v>99</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>66</v>
+      <c r="E19" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="D20" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="F20" s="21" t="s">
         <v>101</v>
       </c>
-      <c r="G20" s="21" t="s">
+      <c r="C20" s="20" t="s">
         <v>102</v>
       </c>
+      <c r="D20" s="20" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="F20" s="20" t="s">
+        <v>105</v>
+      </c>
+      <c r="G20" s="20" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="21">
-      <c r="A21" s="20" t="s">
-        <v>103</v>
-      </c>
-      <c r="B21" s="20" t="s">
-        <v>104</v>
+      <c r="A21" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>108</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="I21" s="17" t="s">
-        <v>109</v>
+        <v>36</v>
+      </c>
+      <c r="I21" s="16" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="8" t="s">
-        <v>110</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>111</v>
-      </c>
-      <c r="C22" s="21" t="s">
-        <v>112</v>
+      <c r="A22" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>115</v>
+      </c>
+      <c r="C22" s="20" t="s">
+        <v>116</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="22"/>
-      <c r="F22" s="22"/>
-      <c r="G22" s="22"/>
+      <c r="E22" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="4" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>14</v>
@@ -1686,312 +1775,312 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="D24" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F24" s="19" t="s">
-        <v>66</v>
+      <c r="E24" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F24" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B25" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>124</v>
+      <c r="A25" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>128</v>
       </c>
       <c r="D25" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="19" t="s">
-        <v>66</v>
+      <c r="E25" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>127</v>
+      <c r="A26" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>131</v>
       </c>
       <c r="D26" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F26" s="19" t="s">
-        <v>66</v>
+      <c r="E26" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="20" t="s">
-        <v>128</v>
-      </c>
-      <c r="B27" s="20" t="s">
-        <v>129</v>
-      </c>
-      <c r="C27" s="21" t="s">
-        <v>130</v>
+      <c r="A27" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>134</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E27" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27" s="19" t="s">
-        <v>66</v>
+      <c r="E27" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="4" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="G28" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="8" t="s">
-        <v>137</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>139</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="E29" s="8" t="s">
+      <c r="A29" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="F29" s="8" t="s">
+      <c r="B29" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="G29" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="I29" s="17" t="s">
+      <c r="C29" s="7" t="s">
         <v>143</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="4" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="20" t="s">
-        <v>149</v>
-      </c>
-      <c r="B31" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="C31" s="21" t="s">
-        <v>151</v>
+      <c r="A31" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>155</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E31" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>66</v>
+      <c r="E31" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="20" t="s">
-        <v>152</v>
-      </c>
-      <c r="B32" s="20" t="s">
-        <v>153</v>
+      <c r="A32" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>157</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="D32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>66</v>
+      <c r="E32" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="20" t="s">
-        <v>155</v>
-      </c>
-      <c r="B33" s="20" t="s">
-        <v>156</v>
+      <c r="A33" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>160</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="D33" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E33" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F33" s="19" t="s">
-        <v>66</v>
+      <c r="E33" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="B34" s="20" t="s">
-        <v>159</v>
-      </c>
-      <c r="C34" s="21" t="s">
-        <v>160</v>
+      <c r="A34" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>164</v>
       </c>
       <c r="D34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E34" s="19" t="s">
-        <v>65</v>
-      </c>
-      <c r="F34" s="19" t="s">
-        <v>66</v>
+      <c r="E34" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F34" s="14" t="s">
+        <v>64</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="B35" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="C35" s="8" t="s">
-        <v>163</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>164</v>
-      </c>
-      <c r="E35" s="8" t="s">
+      <c r="A35" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="B35" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="C35" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="D35" s="7" t="s">
         <v>168</v>
+      </c>
+      <c r="E35" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="F35" s="7" t="s">
+        <v>170</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="H35" s="16" t="s">
+        <v>172</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="5" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="G36" s="5" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="38">
-      <c r="D38" s="6" t="s">
-        <v>175</v>
+      <c r="D38" s="18" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>